<commit_message>
Add 5 percentile for low values
</commit_message>
<xml_diff>
--- a/output/range_output2/Statistics.xlsx
+++ b/output/range_output2/Statistics.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcchanaka/PycharmProjects/Research-Proj-NetEmb/output/range_output2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFABD27D-F1FB-ED4D-A849-6FB6180B96A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C04834-9894-3A44-8760-D25A9CF5C76E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{5F611BA1-94CC-3745-B4FE-A5D1794A1628}"/>
+    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" activeTab="1" xr2:uid="{5F611BA1-94CC-3745-B4FE-A5D1794A1628}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1CDX" sheetId="2" r:id="rId1"/>
+    <sheet name="New-data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>100k</t>
   </si>
@@ -103,13 +104,85 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>1CDX4</t>
+  </si>
+  <si>
+    <t>1CDX3</t>
+  </si>
+  <si>
+    <t>1CDX2</t>
+  </si>
+  <si>
+    <t>1CDX1</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>985/1043</t>
+  </si>
+  <si>
+    <t>956/1043</t>
+  </si>
+  <si>
+    <t>950/1043</t>
+  </si>
+  <si>
+    <t>972/1043</t>
+  </si>
+  <si>
+    <t>678/724</t>
+  </si>
+  <si>
+    <t>660/724</t>
+  </si>
+  <si>
+    <t>651/724</t>
+  </si>
+  <si>
+    <t>654/724</t>
+  </si>
+  <si>
+    <t>1183/1326</t>
+  </si>
+  <si>
+    <t>1150/1326</t>
+  </si>
+  <si>
+    <t>1141/1326</t>
+  </si>
+  <si>
+    <t>1134/1326</t>
+  </si>
+  <si>
+    <t>932/976</t>
+  </si>
+  <si>
+    <t>898/976</t>
+  </si>
+  <si>
+    <t>899/976</t>
+  </si>
+  <si>
+    <t>low-old model</t>
+  </si>
+  <si>
+    <t>low-new model-5%</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +218,27 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,18 +261,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,231 +591,838 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64684C2-6B24-A641-B9E7-CA831A4C9302}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F0CABD-BB3A-CE41-A41D-26838F4BE751}">
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2">
+        <f>899/976</f>
+        <v>0.92110655737704916</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2">
+        <f>898/976</f>
+        <v>0.92008196721311475</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="2">
+        <f>898/976</f>
+        <v>0.92008196721311475</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2">
+        <f>932/976</f>
+        <v>0.95491803278688525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2">
+        <f>1134/1326</f>
+        <v>0.85520361990950222</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2">
+        <f>1141/1326</f>
+        <v>0.86048265460030171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2">
+        <f>1150/1326</f>
+        <v>0.86726998491704377</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="2">
+        <f>1183/1326</f>
+        <v>0.89215686274509809</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2">
+        <f>654/724</f>
+        <v>0.90331491712707179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2">
+        <f>651/724</f>
+        <v>0.899171270718232</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2">
+        <f>660/724</f>
+        <v>0.91160220994475138</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="2">
+        <f>678/724</f>
+        <v>0.93646408839779005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2">
+        <f>972/1043</f>
+        <v>0.93192713326941512</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2">
+        <f>950/1043</f>
+        <v>0.91083413231064236</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2">
+        <f>956/1043</f>
+        <v>0.91658676893576219</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="2">
+        <f>985/1043</f>
+        <v>0.9443911792905082</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
+        <f>899/976</f>
+        <v>0.92110655737704916</v>
+      </c>
+      <c r="D13" s="2">
+        <f>898/976</f>
+        <v>0.92008196721311475</v>
+      </c>
+      <c r="E13" s="2">
+        <f>898/976</f>
+        <v>0.92008196721311475</v>
+      </c>
+      <c r="F13" s="2">
+        <f>932/976</f>
+        <v>0.95491803278688525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2">
+        <f>1134/1326</f>
+        <v>0.85520361990950222</v>
+      </c>
+      <c r="D14" s="2">
+        <f>1141/1326</f>
+        <v>0.86048265460030171</v>
+      </c>
+      <c r="E14" s="2">
+        <f>1150/1326</f>
+        <v>0.86726998491704377</v>
+      </c>
+      <c r="F14" s="2">
+        <f>1183/1326</f>
+        <v>0.89215686274509809</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <f>654/724</f>
+        <v>0.90331491712707179</v>
+      </c>
+      <c r="D15" s="2">
+        <f>651/724</f>
+        <v>0.899171270718232</v>
+      </c>
+      <c r="E15" s="2">
+        <f>660/724</f>
+        <v>0.91160220994475138</v>
+      </c>
+      <c r="F15" s="2">
+        <f>678/724</f>
+        <v>0.93646408839779005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2">
+        <f>972/1043</f>
+        <v>0.93192713326941512</v>
+      </c>
+      <c r="D16" s="2">
+        <f>950/1043</f>
+        <v>0.91083413231064236</v>
+      </c>
+      <c r="E16" s="2">
+        <f>956/1043</f>
+        <v>0.91658676893576219</v>
+      </c>
+      <c r="F16" s="2">
+        <f>985/1043</f>
+        <v>0.9443911792905082</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>977</v>
+      </c>
+      <c r="D20">
+        <v>1652</v>
+      </c>
+      <c r="E20">
+        <v>8045</v>
+      </c>
+      <c r="F20" s="6">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>1327</v>
+      </c>
+      <c r="D21">
+        <v>2580</v>
+      </c>
+      <c r="E21">
+        <v>16810</v>
+      </c>
+      <c r="F21" s="6">
+        <v>7715</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>725</v>
+      </c>
+      <c r="D22">
+        <v>1834</v>
+      </c>
+      <c r="E22">
+        <v>6778</v>
+      </c>
+      <c r="F22" s="6">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>1044</v>
+      </c>
+      <c r="D23">
+        <v>2000</v>
+      </c>
+      <c r="E23">
+        <v>6059</v>
+      </c>
+      <c r="F23" s="6">
+        <v>6059</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>976</v>
+      </c>
+      <c r="D29">
+        <v>1651</v>
+      </c>
+      <c r="E29">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <v>1326</v>
+      </c>
+      <c r="D30">
+        <v>2579</v>
+      </c>
+      <c r="E30">
+        <v>7714</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>724</v>
+      </c>
+      <c r="D31">
+        <v>1833</v>
+      </c>
+      <c r="E31">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>1043</v>
+      </c>
+      <c r="D32">
+        <v>1999</v>
+      </c>
+      <c r="E32">
+        <v>6058</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64684C2-6B24-A641-B9E7-CA831A4C9302}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" customWidth="1"/>
     <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <f>37/37</f>
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f>898/976</f>
         <v>0.92008196721311475</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <f>898/976</f>
         <v>0.92008196721311475</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="2">
         <f>932/976</f>
         <v>0.95491803278688525</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>37</v>
-      </c>
-      <c r="N2">
-        <v>79</v>
-      </c>
-      <c r="O2" s="5">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <f>73/84</f>
         <v>0.86904761904761907</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>75/84</f>
         <v>0.8928571428571429</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <f>75/84</f>
         <v>0.8928571428571429</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="2">
         <f>78/84</f>
         <v>0.9285714285714286</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>84</v>
-      </c>
-      <c r="N3">
-        <v>229</v>
-      </c>
-      <c r="O3" s="5">
-        <v>19824</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <f>31/33</f>
         <v>0.93939393939393945</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f>31/33</f>
         <v>0.93939393939393945</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <f>30/33</f>
         <v>0.90909090909090906</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="2">
         <f>33/33</f>
         <v>1</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4">
-        <v>33</v>
-      </c>
-      <c r="N4">
-        <v>50</v>
-      </c>
-      <c r="O4">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <f>48/51</f>
         <v>0.94117647058823528</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <f>46/51</f>
         <v>0.90196078431372551</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <f>46/51</f>
         <v>0.90196078431372551</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="2">
         <f>47/51</f>
         <v>0.92156862745098034</v>
       </c>
-      <c r="L5" s="6" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+      <c r="D10" s="3">
+        <v>955</v>
+      </c>
+      <c r="E10" s="7">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>84</v>
+      </c>
+      <c r="C11">
+        <v>229</v>
+      </c>
+      <c r="D11" s="3">
+        <v>19824</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>268</v>
+      </c>
+      <c r="E12" s="6">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M5">
+      <c r="B13">
         <v>51</v>
       </c>
-      <c r="N5">
+      <c r="C13">
         <v>51</v>
       </c>
-      <c r="O5">
+      <c r="D13">
         <v>274</v>
+      </c>
+      <c r="E13" s="6">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>175646</v>
+      </c>
+      <c r="C18">
+        <v>20491.25</v>
+      </c>
+      <c r="D18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>176583</v>
+      </c>
+      <c r="C19">
+        <v>34178.618421052597</v>
+      </c>
+      <c r="D19">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>79</v>
+      </c>
+      <c r="D33" s="3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>84</v>
+      </c>
+      <c r="C34">
+        <v>229</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>51</v>
+      </c>
+      <c r="C36">
+        <v>51</v>
+      </c>
+      <c r="D36" s="10">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>